<commit_message>
Updated Sprint 2/3 backlogs
</commit_message>
<xml_diff>
--- a/docs/deliverable 2/Getana_Deliverable_2_SprintBacklog_2.xlsx
+++ b/docs/deliverable 2/Getana_Deliverable_2_SprintBacklog_2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodywilliams/Repositories/RaiderNAV/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodywilliams/Repositories/RaiderNAV/docs/deliverable 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB30CEB-7C44-FE4E-A7C9-DD120BB6AE82}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18300" windowHeight="18000" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="87">
   <si>
     <t>SPRINT BACKLOG — Deliverable 1</t>
   </si>
@@ -231,9 +232,6 @@
     <t>46, Finish focus group document</t>
   </si>
   <si>
-    <t>45, Update daily scrum report daily</t>
-  </si>
-  <si>
     <t>48, Update sprint backlog for beginning of sprint 2</t>
   </si>
   <si>
@@ -243,18 +241,6 @@
     <t>50, Update platform document</t>
   </si>
   <si>
-    <t>51, Update SRS and UCM document</t>
-  </si>
-  <si>
-    <t>53, Create Domain Model and Detailed Design Model document</t>
-  </si>
-  <si>
-    <t>54, Create Configuration Management Plan document</t>
-  </si>
-  <si>
-    <t>55, Create GRL and UCM Models Document</t>
-  </si>
-  <si>
     <t>56, Create user interface for creating a schedule, adding classes, and saving a schedule</t>
   </si>
   <si>
@@ -283,6 +269,24 @@
   </si>
   <si>
     <t>61, Implement front end for route display after API calls to generate route</t>
+  </si>
+  <si>
+    <t>45, Update daily scrum report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In progess as of end of sprint </t>
+  </si>
+  <si>
+    <t>Arpit: 100%</t>
+  </si>
+  <si>
+    <t>Michael, Sakshyam, Vasilis: 100%</t>
+  </si>
+  <si>
+    <t>79, Conduct Focus Group</t>
+  </si>
+  <si>
+    <t>Yong, Vasilis, Arpit, Michael, Sakshyam, Brody: 100%</t>
   </si>
 </sst>
 </file>
@@ -656,7 +660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="134" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="134" zoomScaleNormal="68" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1334,10 +1338,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1442,7 +1446,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -1454,10 +1458,10 @@
         <v>15</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" t="s">
         <v>28</v>
@@ -1465,7 +1469,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -1488,7 +1492,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -1500,12 +1504,18 @@
         <v>15</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
@@ -1517,7 +1527,13 @@
         <v>15</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
@@ -1534,10 +1550,16 @@
         <v>15</v>
       </c>
       <c r="E16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -1551,35 +1573,47 @@
         <v>15</v>
       </c>
       <c r="E17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
       </c>
       <c r="E18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
@@ -1587,141 +1621,149 @@
       <c r="E19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" t="s">
         <v>73</v>
       </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" t="s">
-        <v>14</v>
-      </c>
       <c r="D20" t="s">
         <v>15</v>
       </c>
-      <c r="E20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E20" s="4">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
       </c>
       <c r="E21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>82</v>
+      </c>
+      <c r="G21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
         <v>15</v>
       </c>
       <c r="E22">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D23" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>82</v>
+      </c>
+      <c r="G23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="D24" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" t="s">
-        <v>83</v>
-      </c>
-      <c r="B27" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
-        <v>85</v>
-      </c>
-      <c r="B28" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" t="s">
-        <v>15</v>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>